<commit_message>
duplicate integer array leetcode
</commit_message>
<xml_diff>
--- a/Data Structures and Algo/DS_Algo track.xlsx
+++ b/Data Structures and Algo/DS_Algo track.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t xml:space="preserve">ctrl+m :remove hyperlink</t>
   </si>
@@ -153,7 +153,7 @@
     <t xml:space="preserve">palindrome check</t>
   </si>
   <si>
-    <t xml:space="preserve">loop till hafl length and check the ==
+    <t xml:space="preserve">loop till half length and check the ==
 Editorial: reverse and direct check ==</t>
   </si>
   <si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t xml:space="preserve">learn map method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write a Code to check whether one string is a rotation of another</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concatenate + check substring</t>
   </si>
   <si>
     <t xml:space="preserve">string</t>
@@ -404,7 +410,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,10 +449,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -559,10 +561,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B9" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -741,7 +743,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -759,7 +761,7 @@
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -767,6 +769,14 @@
       </c>
       <c r="E19" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -791,114 +801,114 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="6.42"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="11" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="51.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="11" width="8.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="6.42"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="10" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="10" width="51.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="10" width="8.59"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="11" t="s">
-        <v>49</v>
+      <c r="C2" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>51</v>
+      <c r="C4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>53</v>
+      <c r="D5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="11" t="s">
-        <v>54</v>
+      <c r="D6" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>56</v>
+      <c r="C8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="12" t="s">
-        <v>57</v>
+      <c r="C9" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>61</v>
+      <c r="C11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>63</v>
+      <c r="C13" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C15" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>65</v>
+      <c r="C15" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="14"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>67</v>
+      <c r="C18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>69</v>
+      <c r="C19" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>71</v>
+      <c r="C21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -927,67 +937,67 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="55.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="45.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="55.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="45.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>74</v>
+      <c r="B2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>76</v>
+      <c r="B4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>78</v>
+      <c r="B8" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>80</v>
+      <c r="B11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="16" t="s">
-        <v>81</v>
+      <c r="B12" s="15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="16" t="s">
-        <v>82</v>
+      <c r="B14" s="15" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>84</v>
+      <c r="B16" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
row with max sum
</commit_message>
<xml_diff>
--- a/Data Structures and Algo/DS_Algo track.xlsx
+++ b/Data Structures and Algo/DS_Algo track.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t xml:space="preserve">ctrl+m :remove hyperlink</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t xml:space="preserve">Spiral traversal on a Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search an element in a matriix</t>
   </si>
   <si>
     <t xml:space="preserve">string</t>
@@ -371,15 +377,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color rgb="FF111111"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <u val="single"/>
+      <sz val="9"/>
+      <color rgb="FF111111"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -442,7 +449,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,6 +491,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,10 +612,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C19" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -811,7 +822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -839,6 +850,14 @@
       </c>
       <c r="C22" s="11" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -859,118 +878,118 @@
   </sheetPr>
   <dimension ref="C2:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="6.42"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="12" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="12" width="51.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="12" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="6.42"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="13" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="13" width="51.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="13" width="8.6"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="12" t="s">
-        <v>57</v>
+      <c r="C2" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>59</v>
+      <c r="C4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>61</v>
+      <c r="D5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="12" t="s">
-        <v>62</v>
+      <c r="D6" s="13" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>64</v>
+      <c r="C8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="13" t="s">
-        <v>65</v>
+      <c r="C9" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="C10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>69</v>
+      <c r="C11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>71</v>
+      <c r="C13" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C15" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>73</v>
+      <c r="C15" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="15"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>75</v>
+      <c r="C18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>77</v>
+      <c r="C19" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>79</v>
+      <c r="C21" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -995,71 +1014,71 @@
   </sheetPr>
   <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="55.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="45.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="55.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="45.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>82</v>
+      <c r="B2" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>84</v>
+      <c r="B4" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>86</v>
+      <c r="B8" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>88</v>
+      <c r="B11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="17" t="s">
-        <v>89</v>
+      <c r="B12" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17" t="s">
-        <v>90</v>
+      <c r="B14" s="18" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>92</v>
+      <c r="B16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first and last index of element
</commit_message>
<xml_diff>
--- a/Data Structures and Algo/DS_Algo track.xlsx
+++ b/Data Structures and Algo/DS_Algo track.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="450_curated babbar" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
   <si>
     <t xml:space="preserve">ctrl+m :remove hyperlink</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t xml:space="preserve">Find row with maximum no. of 1's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort matrix</t>
   </si>
   <si>
     <t xml:space="preserve">string</t>
@@ -338,6 +344,13 @@
     <t xml:space="preserve">inside bracked int m is local.. it is initailized again as a local value.
 Correct use is m = 2;
 If not used properly garbage value may be generated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segmentation fault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check return values are provided
+Check out of bound values are called?</t>
   </si>
 </sst>
 </file>
@@ -527,7 +540,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -641,10 +654,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -895,6 +908,14 @@
       </c>
       <c r="C24" s="13" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -930,49 +951,49 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -980,26 +1001,26 @@
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C15" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,26 +1028,26 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1049,13 +1070,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C19"/>
+  <dimension ref="B1:C22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="55.82"/>
@@ -1064,66 +1085,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="20"/>
     </row>
     <row r="2" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="21" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="81.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missing and repeating number
</commit_message>
<xml_diff>
--- a/Data Structures and Algo/DS_Algo track.xlsx
+++ b/Data Structures and Algo/DS_Algo track.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="450_curated babbar" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="115">
   <si>
     <t xml:space="preserve">ctrl+m :remove hyperlink</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t xml:space="preserve">Search in a rotated sorted array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 feb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle of Three </t>
+  </si>
+  <si>
+    <t xml:space="preserve">square root of an integer</t>
   </si>
   <si>
     <t xml:space="preserve">string</t>
@@ -393,7 +402,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -417,7 +426,7 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -432,39 +441,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF111111"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF111111"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
       <sz val="9"/>
       <color rgb="FF111111"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -527,7 +505,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -552,14 +530,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -568,7 +538,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -576,35 +546,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -702,10 +664,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -723,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -751,7 +713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="true" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="3" customFormat="true" ht="29.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -762,7 +724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="true" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="3" customFormat="true" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="D6" s="3" t="s">
         <v>12</v>
@@ -771,7 +733,7 @@
     <row r="7" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" s="3" customFormat="true" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="3" customFormat="true" ht="29.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -782,7 +744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="true" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="3" customFormat="true" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -793,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="true" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="3" customFormat="true" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="C10" s="3" t="s">
         <v>19</v>
@@ -802,14 +764,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="true" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="3" customFormat="true" ht="29.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
-      <c r="C11" s="6"/>
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="true" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="3" customFormat="true" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -823,11 +784,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -844,7 +805,7 @@
       <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -869,7 +830,7 @@
       <c r="D16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -884,7 +845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -902,7 +863,7 @@
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -912,7 +873,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -927,7 +888,7 @@
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -938,7 +899,7 @@
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>56</v>
       </c>
     </row>
@@ -946,7 +907,7 @@
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="8" t="s">
         <v>58</v>
       </c>
     </row>
@@ -954,7 +915,7 @@
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -970,7 +931,7 @@
       <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -978,8 +939,21 @@
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="8" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1006,112 +980,112 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="6.42"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="15" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="15" width="51.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="15" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="6.42"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="11" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="51.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="11" width="8.6"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="15" t="s">
-        <v>65</v>
+      <c r="C2" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>67</v>
+      <c r="C4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>69</v>
+      <c r="D5" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="15" t="s">
-        <v>70</v>
+      <c r="D6" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>72</v>
+      <c r="C8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="16" t="s">
-        <v>73</v>
+      <c r="C9" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="C10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>77</v>
+      <c r="C11" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>79</v>
+      <c r="C13" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C15" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>81</v>
+      <c r="C15" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="18"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>83</v>
+      <c r="C18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>85</v>
+      <c r="C19" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>87</v>
+      <c r="C21" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1136,120 +1110,120 @@
   </sheetPr>
   <dimension ref="B1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="55.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="45.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="55.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="45.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="B1" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>90</v>
+      <c r="B2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>92</v>
+      <c r="B4" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>94</v>
+      <c r="B8" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>96</v>
+      <c r="B11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="20" t="s">
-        <v>97</v>
+      <c r="B12" s="16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="20" t="s">
-        <v>98</v>
+      <c r="B14" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>100</v>
+      <c r="B16" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="81.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>102</v>
+      <c r="B19" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>104</v>
+      <c r="B22" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C24" s="23" t="s">
-        <v>105</v>
+      <c r="C24" s="19" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>107</v>
+      <c r="B25" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="23" t="s">
-        <v>108</v>
+      <c r="C26" s="19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="23" t="s">
-        <v>109</v>
+      <c r="C27" s="19" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="23" t="s">
-        <v>110</v>
+      <c r="C28" s="19" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="23" t="s">
-        <v>111</v>
+      <c r="C29" s="19" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>